<commit_message>
Improved the main layer of logic for the formation of estimates
</commit_message>
<xml_diff>
--- a/dispatcher/src/main/resources/basis.xlsx
+++ b/dispatcher/src/main/resources/basis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\java_progects\auto_estimator\auto_estimator\dispatcher\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B26BAC1-2CC7-4511-8265-5780EF5ABDDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C085733-2D85-4F18-AE97-8FD7D74F79D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="25815" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="450" windowWidth="25815" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Смета" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
     <t>Контакты: +375 29 676-28-71 info@kaminsky.by</t>
   </si>
   <si>
-    <t>Гарантийные обязательства  - 2 года гарантии. (Возможно послегарантийное обслуживание)</t>
-  </si>
-  <si>
     <t>Заказчик: _____________</t>
   </si>
   <si>
@@ -46,6 +43,9 @@
   </si>
   <si>
     <t>Наименование работы</t>
+  </si>
+  <si>
+    <t>Гарантийные обязательства  - 2 года гарантии (возможно послегарантийное обслуживание)</t>
   </si>
 </sst>
 </file>
@@ -142,7 +142,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor rgb="FFF0C8A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -430,6 +430,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF0C8A0"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -764,7 +769,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A4" sqref="A4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -800,12 +805,12 @@
       <c r="E2" s="17"/>
       <c r="F2" s="18"/>
       <c r="G2" s="4">
-        <v>2.64</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B3" s="20"/>
       <c r="C3" s="20"/>
@@ -816,7 +821,7 @@
     </row>
     <row r="4" spans="1:7" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="23"/>
       <c r="C4" s="23"/>
@@ -827,7 +832,7 @@
     </row>
     <row r="5" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="26"/>
       <c r="C5" s="26"/>
@@ -855,7 +860,7 @@
     </row>
     <row r="8" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>

</xml_diff>